<commit_message>
docgen width 문제 해결
</commit_message>
<xml_diff>
--- a/Common/doc/docgen/media/table_sample.xlsx
+++ b/Common/doc/docgen/media/table_sample.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Project\Profiles\Qualitas\Documents\docgen\media\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\Profiles\Common\doc\docgen\media\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65915DEA-13B2-430A-84DA-6005DA2A12DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9CD3864-81DD-4750-8F53-F24471BE52A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3072" yWindow="2304" windowWidth="21528" windowHeight="7476" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3435" yWindow="1380" windowWidth="18465" windowHeight="7335" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -51,9 +51,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>description #1</t>
-  </si>
-  <si>
     <t>description #6</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -78,19 +75,84 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>*Name</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>*Index</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>description #2</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>@&lt;b&gt;description @&lt;color:FF0000&gt;#3@&lt;/color&gt;@&lt;/b&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">description #1 bold </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>colored</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">italic </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>underline</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Index</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -98,7 +160,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -108,6 +170,44 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="맑은 고딕"/>
       <family val="3"/>
       <charset val="129"/>
@@ -134,17 +234,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -428,29 +532,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="10" customWidth="1"/>
-    <col min="2" max="2" width="10.59765625" customWidth="1"/>
-    <col min="3" max="3" width="50.8984375" customWidth="1"/>
+    <col min="2" max="2" width="10.625" customWidth="1"/>
+    <col min="3" max="3" width="50.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -458,52 +560,52 @@
         <v>1</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A4" s="3">
+      <c r="C3" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="6">
         <v>2</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="4" t="s">
         <v>3</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A5" s="3"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="6"/>
       <c r="B5" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.4">
+        <v>10</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>3</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>4</v>
       </c>
@@ -511,10 +613,10 @@
         <v>4</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.4">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>5</v>
       </c>
@@ -522,7 +624,7 @@
         <v>5</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
codgen 엑셀 cell fill 조건 수정
</commit_message>
<xml_diff>
--- a/Common/doc/docgen/media/table_sample.xlsx
+++ b/Common/doc/docgen/media/table_sample.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\Profiles\Common\doc\docgen\media\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9CD3864-81DD-4750-8F53-F24471BE52A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E41AAA4-AE8A-40B5-8CEB-392FC91BA453}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3435" yWindow="1380" windowWidth="18465" windowHeight="7335" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="37860" yWindow="1185" windowWidth="11475" windowHeight="7530" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -160,7 +160,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -213,13 +213,44 @@
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00B0F0"/>
+      <name val="맑은 고딕"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -234,7 +265,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -250,6 +281,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
@@ -532,7 +573,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
@@ -556,7 +599,7 @@
       <c r="A2" s="1">
         <v>0</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="7" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="2" t="s">
@@ -567,7 +610,7 @@
       <c r="A3" s="1">
         <v>1</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="8" t="s">
         <v>2</v>
       </c>
       <c r="C3" s="5" t="s">
@@ -587,7 +630,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="6"/>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="9" t="s">
         <v>10</v>
       </c>
       <c r="C5" s="3" t="s">
@@ -612,7 +655,7 @@
       <c r="B7" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="10" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>